<commit_message>
Updated readMovie to column based
</commit_message>
<xml_diff>
--- a/src/database/Movies.xlsx
+++ b/src/database/Movies.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SC2002_Assignment\src\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9601FD-8258-4C01-A2A6-D7E0F5E548F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA38FDE-4E0F-4149-A11E-A20D9609FCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Dance all night</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Star</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>1</t>
@@ -144,7 +141,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -500,16 +496,16 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
-    <col min="4" max="4" customWidth="true" style="1" width="13.0"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -522,23 +518,23 @@
       <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>32</v>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -551,23 +547,23 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>33</v>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -580,23 +576,23 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>33</v>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -609,23 +605,23 @@
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -638,52 +634,52 @@
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>33</v>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -696,20 +692,20 @@
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>33</v>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insert,Update Done but minor bugs(validation)
</commit_message>
<xml_diff>
--- a/src/database/Movies.xlsx
+++ b/src/database/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SC2002_Assignment\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9601FD-8258-4C01-A2A6-D7E0F5E548F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C60483-E130-4595-BAC2-B53E5A5316BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
-  <si>
-    <t>Dance all night</t>
-  </si>
-  <si>
-    <t>Freedom</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Dog life</t>
   </si>
@@ -65,79 +59,67 @@
     <t>Showing</t>
   </si>
   <si>
+    <t>Dog live life</t>
+  </si>
+  <si>
+    <t>Age Rating</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>New Chance</t>
+  </si>
+  <si>
+    <t>New Hope</t>
+  </si>
+  <si>
+    <t>Coming Soon</t>
+  </si>
+  <si>
     <t>M13</t>
   </si>
   <si>
-    <t>dancing people dancing</t>
-  </si>
-  <si>
-    <t>Freedom is a lie</t>
-  </si>
-  <si>
-    <t>Dog live life</t>
-  </si>
-  <si>
-    <t>Age Rating</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Horror</t>
-  </si>
-  <si>
-    <t>Comedy</t>
-  </si>
-  <si>
-    <t>Sad</t>
-  </si>
-  <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Shoe Michael</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Star</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>P</t>
+    <t/>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>Test 2.0</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test 3.0</t>
+  </si>
+  <si>
+    <t>Test 30.</t>
+  </si>
+  <si>
+    <t>InsertTest</t>
+  </si>
+  <si>
+    <t>INserta</t>
   </si>
 </sst>
 </file>
@@ -174,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,6 +165,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,216 +483,216 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
-    <col min="4" max="4" customWidth="true" style="1" width="13.0"/>
+    <col min="3" max="3" customWidth="true" style="1" width="13.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
         <v>3</v>
       </c>
-      <c r="B1" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2">
+      <c r="D1" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E1" s="4">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0">
+        <v>8</v>
+      </c>
+      <c r="I1" t="n" s="0">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="B2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s" s="0">
+      <c r="B3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="G1" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>32</v>
+      <c r="E3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>33</v>
+      <c r="B4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" t="s" s="0">
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
+      <c r="D5" t="s" s="0">
+        <v>5</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s" s="0">
+      <c r="H6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update movielistUI to not show 'End of Showing' movies
</commit_message>
<xml_diff>
--- a/src/database/Movies.xlsx
+++ b/src/database/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F4B76F-6F09-4788-9FBD-D5348B35AA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBFDFB2-ADA2-43E1-ADEA-50BAEDA35F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>NC16</t>
   </si>
   <si>
-    <t>PG13</t>
-  </si>
-  <si>
     <t>R21</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Overall Reviewer Rating</t>
+  </si>
+  <si>
+    <t>End of Showing</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -674,10 +674,10 @@
         <v>31</v>
       </c>
       <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
@@ -688,28 +688,28 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,10 +717,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -769,25 +769,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>-1</v>

</xml_diff>